<commit_message>
Removed New, Custom & Special textures
1. All BD64 maps purged of obsolete textures.
2. Terrain file updated.
3. GLDefs files updated.
</commit_message>
<xml_diff>
--- a/Reference_Info/Texture replacements.xlsx
+++ b/Reference_Info/Texture replacements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stevenconnell\OneDrive - CTS Group Pty Ltd\Documents\GitHub\BD64maps_v2.666\Reference_Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC3E3EB-2563-42AC-A3AB-94EFC5B98B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9588EEFE-37EB-4317-8891-5F0B19E8FCA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="1635" windowWidth="20040" windowHeight="11295" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
+    <workbookView xWindow="5310" yWindow="2520" windowWidth="20040" windowHeight="11295" xr2:uid="{A567E191-AF02-4B5D-A98D-30E219FAA09A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -830,7 +830,7 @@
   <dimension ref="A1:E109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D61" sqref="A61:D61"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>